<commit_message>
added input for csv file
</commit_message>
<xml_diff>
--- a/cherry fly ids.xlsx
+++ b/cherry fly ids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicCage\Desktop\walnut_wol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NicCage\Box\wolbachia\walnut_wolbachia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68C600F-FCD4-4A24-91F2-17320124F82A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398B776-6B9E-4289-8749-6943655336B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BA95FFA-1C86-4E5C-B660-CEEB5540E083}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5BA95FFA-1C86-4E5C-B660-CEEB5540E083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,12 +127,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,8 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +473,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +505,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -554,7 +561,7 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
     </row>
@@ -568,7 +575,7 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>6</v>
       </c>
     </row>
@@ -610,7 +617,7 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>9</v>
       </c>
     </row>
@@ -624,7 +631,7 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>10</v>
       </c>
     </row>
@@ -638,7 +645,7 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>11</v>
       </c>
     </row>
@@ -652,7 +659,7 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>12</v>
       </c>
     </row>
@@ -666,7 +673,7 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>13</v>
       </c>
     </row>
@@ -680,7 +687,7 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>14</v>
       </c>
     </row>
@@ -694,7 +701,7 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>15</v>
       </c>
     </row>
@@ -708,7 +715,7 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>16</v>
       </c>
     </row>
@@ -722,7 +729,7 @@
       <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>17</v>
       </c>
     </row>
@@ -736,7 +743,7 @@
       <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>18</v>
       </c>
     </row>
@@ -750,7 +757,7 @@
       <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>19</v>
       </c>
     </row>
@@ -778,7 +785,7 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>21</v>
       </c>
     </row>

</xml_diff>